<commit_message>
grade update: midterm 2
</commit_message>
<xml_diff>
--- a/Grades/Grades.xlsx
+++ b/Grades/Grades.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
   <si>
     <t xml:space="preserve">First name</t>
   </si>
@@ -32,6 +32,9 @@
   </si>
   <si>
     <t xml:space="preserve">Midterm 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Midterm 2</t>
   </si>
   <si>
     <t xml:space="preserve">Will</t>
@@ -232,13 +235,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F11" activeCellId="0" sqref="F11"/>
+      <selection pane="topLeft" activeCell="G10" activeCellId="0" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.50390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.51171875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="9.68"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -250,173 +256,196 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="1" t="s">
         <v>3</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="F2" s="1" t="n">
         <f aca="false">0</f>
         <v>0</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F3" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="F3" s="1" t="n">
         <f aca="false">50/50</f>
         <v>1</v>
+      </c>
+      <c r="G3" s="0" t="n">
+        <f aca="false">58/60</f>
+        <v>0.966666666666667</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F4" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="F4" s="1" t="n">
         <f aca="false">49/50</f>
         <v>0.98</v>
       </c>
+      <c r="G4" s="0" t="n">
+        <f aca="false">57/60</f>
+        <v>0.95</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F5" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="F5" s="1" t="n">
         <f aca="false">50/50</f>
         <v>1</v>
+      </c>
+      <c r="G5" s="0" t="n">
+        <f aca="false">58/60</f>
+        <v>0.966666666666667</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F6" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="F6" s="1" t="n">
         <f aca="false">50/50</f>
         <v>1</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F7" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="F7" s="1" t="n">
         <f aca="false">50/50</f>
         <v>1</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F8" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="F8" s="1" t="n">
         <f aca="false">0</f>
         <v>0</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F9" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="F9" s="1" t="n">
         <f aca="false">45/50</f>
         <v>0.9</v>
       </c>
+      <c r="G9" s="0" t="n">
+        <f aca="false">60/60</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="F10" s="0" t="n">
+        <v>31</v>
+      </c>
+      <c r="F10" s="1" t="n">
         <f aca="false">0</f>
         <v>0</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="F11" s="0" t="n">
+        <v>34</v>
+      </c>
+      <c r="F11" s="1" t="n">
         <f aca="false">46/50</f>
         <v>0.92</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="F12" s="0" t="n">
+        <v>37</v>
+      </c>
+      <c r="F12" s="1" t="n">
         <f aca="false">50/50</f>
         <v>1</v>
+      </c>
+      <c r="G12" s="0" t="n">
+        <f aca="false">55/60</f>
+        <v>0.916666666666667</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
grade update: scientific essays
</commit_message>
<xml_diff>
--- a/Grades/Grades.xlsx
+++ b/Grades/Grades.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t xml:space="preserve">First name</t>
   </si>
@@ -35,6 +35,9 @@
   </si>
   <si>
     <t xml:space="preserve">Midterm 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Science Paper</t>
   </si>
   <si>
     <t xml:space="preserve">Will</t>
@@ -226,15 +229,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G11" activeCellId="0" sqref="G11"/>
+      <selection pane="topLeft" activeCell="H10" activeCellId="0" sqref="H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.53125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="9.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="12.3"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -253,16 +259,19 @@
       <c r="G1" s="0" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H1" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F2" s="1" t="n">
         <f aca="false">0</f>
@@ -272,16 +281,20 @@
         <f aca="false">0</f>
         <v>0</v>
       </c>
+      <c r="H2" s="0" t="n">
+        <f aca="false">0/100</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F3" s="1" t="n">
         <f aca="false">50/50</f>
@@ -291,16 +304,20 @@
         <f aca="false">58/60</f>
         <v>0.966666666666667</v>
       </c>
+      <c r="H3" s="0" t="n">
+        <f aca="false">100/100</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F4" s="1" t="n">
         <f aca="false">49/50</f>
@@ -310,16 +327,20 @@
         <f aca="false">57/60</f>
         <v>0.95</v>
       </c>
+      <c r="H4" s="0" t="n">
+        <f aca="false">0.9</f>
+        <v>0.9</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F5" s="1" t="n">
         <f aca="false">50/50</f>
@@ -329,16 +350,20 @@
         <f aca="false">58/60</f>
         <v>0.966666666666667</v>
       </c>
+      <c r="H5" s="0" t="n">
+        <f aca="false">0.9</f>
+        <v>0.9</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F6" s="1" t="n">
         <f aca="false">50/50</f>
@@ -351,13 +376,13 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F7" s="1" t="n">
         <f aca="false">50/50</f>
@@ -370,13 +395,13 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F8" s="1" t="n">
         <f aca="false">0</f>
@@ -386,16 +411,20 @@
         <f aca="false">59/60</f>
         <v>0.983333333333333</v>
       </c>
+      <c r="H8" s="0" t="n">
+        <f aca="false">0.93</f>
+        <v>0.93</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F9" s="1" t="n">
         <f aca="false">45/50</f>
@@ -405,16 +434,20 @@
         <f aca="false">60/60</f>
         <v>1</v>
       </c>
+      <c r="H9" s="0" t="n">
+        <f aca="false">1</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F10" s="1" t="n">
         <f aca="false">46/50</f>
@@ -427,13 +460,13 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F11" s="1" t="n">
         <f aca="false">50/50</f>
@@ -442,6 +475,10 @@
       <c r="G11" s="0" t="n">
         <f aca="false">55/60</f>
         <v>0.916666666666667</v>
+      </c>
+      <c r="H11" s="0" t="n">
+        <f aca="false">95/100</f>
+        <v>0.95</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
grade update ... two students remaining
</commit_message>
<xml_diff>
--- a/Grades/Grades.xlsx
+++ b/Grades/Grades.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="45">
   <si>
     <t xml:space="preserve">First name</t>
   </si>
@@ -64,7 +64,7 @@
     <t xml:space="preserve">wgearhar@poets.whittier.edu</t>
   </si>
   <si>
-    <t xml:space="preserve">F</t>
+    <t xml:space="preserve">D+</t>
   </si>
   <si>
     <t xml:space="preserve">Arnau</t>
@@ -106,6 +106,9 @@
     <t xml:space="preserve">lgrey@poets.whittier.edu</t>
   </si>
   <si>
+    <t xml:space="preserve">??</t>
+  </si>
+  <si>
     <t xml:space="preserve">Esiete Yismaw</t>
   </si>
   <si>
@@ -113,6 +116,9 @@
   </si>
   <si>
     <t xml:space="preserve">emebrati@poets.whittier.edu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B-</t>
   </si>
   <si>
     <t xml:space="preserve">Dary</t>
@@ -253,10 +259,10 @@
   <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I10" activeCellId="0" sqref="I10"/>
+      <selection pane="topLeft" activeCell="I11" activeCellId="0" sqref="I11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.58203125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.91"/>
@@ -509,16 +515,19 @@
         <f aca="false">K6+0.03</f>
         <v>0.626666666666667</v>
       </c>
+      <c r="M6" s="0" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F7" s="1" t="n">
         <f aca="false">50/50</f>
@@ -548,20 +557,23 @@
         <f aca="false">K7+0.03</f>
         <v>0.806666666666667</v>
       </c>
+      <c r="M7" s="0" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="F8" s="1" t="n">
-        <f aca="false">0</f>
-        <v>0</v>
+        <f aca="false">43/50</f>
+        <v>0.86</v>
       </c>
       <c r="G8" s="0" t="n">
         <f aca="false">59/60</f>
@@ -581,22 +593,25 @@
       </c>
       <c r="K8" s="0" t="n">
         <f aca="false">0.2*F8+0.2*G8+0.2*H8+0.2*I8+0.2*J8</f>
-        <v>0.776666666666667</v>
+        <v>0.948666666666666</v>
       </c>
       <c r="L8" s="0" t="n">
         <f aca="false">K8+0.03</f>
-        <v>0.806666666666667</v>
+        <v>0.978666666666667</v>
+      </c>
+      <c r="M8" s="0" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="F9" s="1" t="n">
         <f aca="false">45/50</f>
@@ -632,29 +647,29 @@
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="F10" s="1" t="n">
         <f aca="false">46/50</f>
         <v>0.92</v>
       </c>
       <c r="G10" s="0" t="n">
-        <f aca="false">0</f>
-        <v>0</v>
+        <f aca="false">50/60</f>
+        <v>0.833333333333333</v>
       </c>
       <c r="H10" s="0" t="n">
-        <f aca="false">0</f>
-        <v>0</v>
+        <f aca="false">40/100</f>
+        <v>0.4</v>
       </c>
       <c r="I10" s="0" t="n">
-        <f aca="false">0</f>
-        <v>0</v>
+        <f aca="false">1</f>
+        <v>1</v>
       </c>
       <c r="J10" s="0" t="n">
         <f aca="false">1</f>
@@ -662,22 +677,25 @@
       </c>
       <c r="K10" s="0" t="n">
         <f aca="false">0.2*F10+0.2*G10+0.2*H10+0.2*I10+0.2*J10</f>
-        <v>0.384</v>
+        <v>0.830666666666667</v>
       </c>
       <c r="L10" s="0" t="n">
         <f aca="false">K10+0.03</f>
-        <v>0.414</v>
+        <v>0.860666666666667</v>
+      </c>
+      <c r="M10" s="0" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="F11" s="1" t="n">
         <f aca="false">50/50</f>

</xml_diff>